<commit_message>
Code updated 23-03-25 11:30:58
</commit_message>
<xml_diff>
--- a/Season_Trophies/86.xlsx
+++ b/Season_Trophies/86.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E164"/>
+  <dimension ref="A1:E165"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -396,7 +396,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>45734</t>
+          <t>45710</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -416,24 +416,24 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>3570</t>
+          <t>3664</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>108</t>
+          <t>455</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>26424998</t>
+          <t>32613475</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>"Smok3y 1nOnly"</t>
+          <t>"李 无 善 德"</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -443,24 +443,24 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>7349</t>
+          <t>7481</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>727</t>
+          <t>705</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>32613475</t>
+          <t>6940556</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>"李 无 善 德"</t>
+          <t>"Cry ab it林黛玉ᶻᵍˣ"</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -470,24 +470,24 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>7088</t>
+          <t>7385</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>913</t>
+          <t>925</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>6940556</t>
+          <t>26424998</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>"Cry ab it林黛玉ᶻᵍˣ"</t>
+          <t>"Smok3y 1nOnly"</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -497,14 +497,14 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>7027</t>
+          <t>7318</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>1687</t>
+          <t>3158</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -524,14 +524,14 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>6839</t>
+          <t>6817</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>7577</t>
+          <t>9615</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -551,14 +551,14 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>5977</t>
+          <t>5955</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>201</t>
+          <t>214</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -578,14 +578,14 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>7304</t>
+          <t>7589</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>737</t>
+          <t>1160</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -605,14 +605,14 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>7081</t>
+          <t>7252</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>802</t>
+          <t>1367</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -632,14 +632,14 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>7061</t>
+          <t>7192</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>3221</t>
+          <t>2955</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -659,24 +659,24 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>6545</t>
+          <t>6858</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>9522</t>
+          <t>8883</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>21665473</t>
+          <t>43800641</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>"Dog Gamedesiger"</t>
+          <t>㊥蛋蛋大</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -686,14 +686,14 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>5767</t>
+          <t>6028</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>9647</t>
+          <t>9742</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -713,24 +713,24 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>5753</t>
+          <t>5942</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>11253</t>
+          <t>11270</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>43800641</t>
+          <t>21665473</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>㊥蛋蛋大</t>
+          <t>"Dog Gamedesiger"</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -740,14 +740,14 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>5606</t>
+          <t>5785</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>12931</t>
+          <t>12520</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -767,14 +767,14 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>5465</t>
+          <t>5659</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>29</t>
+          <t>166</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -794,24 +794,24 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>7388</t>
+          <t>7607</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2281</t>
+          <t>1912</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>46422609</t>
+          <t>31267627</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>㊥林天大大神</t>
+          <t>"㊥ Martin"</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -821,24 +821,24 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>6712</t>
+          <t>7060</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2360</t>
+          <t>2240</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>1820342</t>
+          <t>25376635</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>摸鱼爱好者三战</t>
+          <t>"sanchez ᶻᵍˣ"</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -848,24 +848,24 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>6697</t>
+          <t>6997</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2575</t>
+          <t>2403</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>31267627</t>
+          <t>1820342</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>"㊥ Martin"</t>
+          <t>摸鱼爱好者三战</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -875,24 +875,24 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>6652</t>
+          <t>6961</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2679</t>
+          <t>2464</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>25376635</t>
+          <t>46422609</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>"sanchez ᶻᵍˣ"</t>
+          <t>㊥林天大大神</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -902,14 +902,14 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>6635</t>
+          <t>6947</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>3374</t>
+          <t>3152</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -929,24 +929,24 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>6520</t>
+          <t>6818</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>3546</t>
+          <t>4080</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>21735478</t>
+          <t>3477306</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>耀翔fly</t>
+          <t>"MeGa Tsai"</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -956,24 +956,24 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>6490</t>
+          <t>6647</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>4319</t>
+          <t>4477</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>3477306</t>
+          <t>21735478</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>"MeGa Tsai"</t>
+          <t>耀翔fly</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -983,24 +983,24 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>6367</t>
+          <t>6585</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>4687</t>
+          <t>5055</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>38711610</t>
+          <t>26280580</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>心灵有为</t>
+          <t>AOW全体工作人员吃屎交易大厅</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -1010,24 +1010,24 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>6312</t>
+          <t>6491</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>5068</t>
+          <t>5165</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>9541747</t>
+          <t>30411791</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>豹子头林冲</t>
+          <t>"㊥Ⓩ GOÐAFRÆÐI ᶻᵍˣ"</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -1037,24 +1037,24 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>6264</t>
+          <t>6476</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>5085</t>
+          <t>5252</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>26588375</t>
+          <t>33656016</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>何苦僧ai</t>
+          <t>㊥☆梅海听雪☆</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -1064,24 +1064,24 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>6262</t>
+          <t>6461</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>4994</t>
+          <t>5312</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>6510348</t>
+          <t>28749280</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Bonpoisson</t>
+          <t>㊥老船⛵⛵</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -1091,24 +1091,24 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>6273</t>
+          <t>6452</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>5149</t>
+          <t>5464</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>33656016</t>
+          <t>38711610</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>㊥☆梅海听雪☆</t>
+          <t>心灵有为</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -1118,24 +1118,24 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>6254</t>
+          <t>6429</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>5358</t>
+          <t>5594</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>30411791</t>
+          <t>6510348</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>"㊥Ⓩ GOÐAFRÆÐI ᶻᵍˣ"</t>
+          <t>Bonpoisson</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -1145,24 +1145,24 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>6229</t>
+          <t>6414</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>5470</t>
+          <t>5158</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>28749280</t>
+          <t>9541747</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>㊥老船⛵⛵</t>
+          <t>豹子头林冲</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -1172,24 +1172,24 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>6216</t>
+          <t>6476</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>5537</t>
+          <t>6665</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>44955827</t>
+          <t>31217211</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>丶小阿狸丿</t>
+          <t>解憂雜貨鋪㊥</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -1199,24 +1199,24 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>6206</t>
+          <t>6276</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>6750</t>
+          <t>7458</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>26280580</t>
+          <t>29729468</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>AOW全体工作人员吃屎交易大厅</t>
+          <t>"风神舞动 WDᶻᵍˣ"</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -1226,24 +1226,24 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>6063</t>
+          <t>6179</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>8093</t>
+          <t>8301</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>29729468</t>
+          <t>44955827</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>"风神舞动 WDᶻᵍˣ"</t>
+          <t>丶小阿狸丿</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -1253,14 +1253,14 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>5917</t>
+          <t>6083</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>12821</t>
+          <t>13190</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -1280,14 +1280,14 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>5474</t>
+          <t>5595</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>12544</t>
+          <t>14118</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -1307,14 +1307,14 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>5497</t>
+          <t>5515</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>15830</t>
+          <t>16054</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -1334,14 +1334,14 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>5257</t>
+          <t>5375</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>17504</t>
+          <t>17507</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -1361,14 +1361,14 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>5154</t>
+          <t>5288</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>20041</t>
+          <t>21724</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -1388,14 +1388,14 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>5007</t>
+          <t>5027</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>21300</t>
+          <t>23366</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -1422,17 +1422,17 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>26668</t>
+          <t>24796</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>32929656</t>
+          <t>46289694</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>"EIH Wilson Chu"</t>
+          <t>㊥Vincent</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
@@ -1442,24 +1442,24 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>4663</t>
+          <t>4849</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>48466</t>
+          <t>26409</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>7587898</t>
+          <t>32929656</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>藍精靈ᶻᵍˣ</t>
+          <t>"EIH Wilson Chu"</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -1469,24 +1469,24 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>3336</t>
+          <t>4768</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>65982</t>
+          <t>49331</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>47928278</t>
+          <t>7587898</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>"落日幻影 哈哈哈"</t>
+          <t>藍精靈ᶻᵍˣ</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
@@ -1496,24 +1496,24 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>2548</t>
+          <t>3336</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>999999</t>
+          <t>66757</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>23687250</t>
+          <t>47928278</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>"jetlijp ᶻᵍˣ"</t>
+          <t>"落日幻影 哈哈哈"</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
@@ -1523,51 +1523,51 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2548</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>1770</t>
+          <t>999999</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>27484940</t>
+          <t>23687250</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>66666zgx</t>
+          <t>"jetlijp ᶻᵍˣ"</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>一馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>6821</t>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>18419</t>
+          <t>2780</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>38809086</t>
+          <t>27484940</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Kouenᶻᵍˣ</t>
+          <t>66666zgx</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -1577,24 +1577,24 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>5098</t>
+          <t>6888</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>6063</t>
+          <t>19258</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>13738844</t>
+          <t>38809086</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>"Chen Hao"</t>
+          <t>Kouenᶻᵍˣ</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -1604,24 +1604,24 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>6144</t>
+          <t>5184</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>10418</t>
+          <t>6223</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>42434117</t>
+          <t>13738844</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>㊥有双飞鸟</t>
+          <t>"Chen Hao"</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
@@ -1631,24 +1631,24 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>5680</t>
+          <t>6333</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>10449</t>
+          <t>9262</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>49710892</t>
+          <t>42434117</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>MMMMMMM</t>
+          <t>㊥有双飞鸟</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
@@ -1658,14 +1658,14 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>5677</t>
+          <t>5998</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>10647</t>
+          <t>11780</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -1685,24 +1685,24 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>5662</t>
+          <t>5732</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>12440</t>
+          <t>12413</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>53520939</t>
+          <t>49710892</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>㊥虎哥tiger</t>
+          <t>MMMMMMM</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
@@ -1712,24 +1712,24 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>5505</t>
+          <t>5668</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>14752</t>
+          <t>12888</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>4756174</t>
+          <t>53520939</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>純希です</t>
+          <t>㊥虎哥tiger</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
@@ -1739,14 +1739,14 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>5328</t>
+          <t>5623</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>15829</t>
+          <t>15808</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -1766,14 +1766,14 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>5257</t>
+          <t>5392</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>16047</t>
+          <t>17343</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -1793,24 +1793,24 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>5245</t>
+          <t>5298</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>25760</t>
+          <t>18873</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>55769051</t>
+          <t>4756174</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>㊥叮叮当.</t>
+          <t>純希です</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
@@ -1820,24 +1820,24 @@
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>4705</t>
+          <t>5206</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>999999</t>
+          <t>23344</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>43812707</t>
+          <t>55769051</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>bbtt</t>
+          <t>㊥叮叮当.</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
@@ -1847,24 +1847,24 @@
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>4932</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>720</t>
+          <t>999999</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>8741713</t>
+          <t>43812707</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t xml:space="preserve">㊥大咖玩家ky </t>
+          <t>bbtt</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
@@ -1874,14 +1874,14 @@
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>7090</t>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>1383</t>
+          <t>1109</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -1901,24 +1901,24 @@
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>6909</t>
+          <t>7267</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>2325</t>
+          <t>1144</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>29211638</t>
+          <t>8741713</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>"㊥ PhononDisperse"</t>
+          <t xml:space="preserve">㊥大咖玩家ky </t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
@@ -1928,24 +1928,24 @@
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>6703</t>
+          <t>7257</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>4456</t>
+          <t>1671</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>16206490</t>
+          <t>29211638</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>㊥Godcys</t>
+          <t>"㊥ PhononDisperse"</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
@@ -1955,24 +1955,24 @@
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>6346</t>
+          <t>7117</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>7122</t>
+          <t>4341</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>4493731</t>
+          <t>26588375</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>Player-1527362</t>
+          <t>何苦僧ai</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
@@ -1982,24 +1982,24 @@
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>6025</t>
+          <t>6603</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>7226</t>
+          <t>4418</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>7852598</t>
+          <t>16206490</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>seiji</t>
+          <t>㊥Godcys</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
@@ -2009,24 +2009,24 @@
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>6014</t>
+          <t>6591</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>9535</t>
+          <t>6811</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>31217211</t>
+          <t>4493731</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>解憂雜貨鋪㊥</t>
+          <t>Player-1527362</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
@@ -2036,24 +2036,24 @@
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>5765</t>
+          <t>6258</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>10363</t>
+          <t>7547</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>47131129</t>
+          <t>7852598</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>NAM</t>
+          <t>seiji</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
@@ -2063,24 +2063,24 @@
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>5686</t>
+          <t>6168</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>10461</t>
+          <t>9801</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>22885399</t>
+          <t>47131129</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>余文琪</t>
+          <t>NAM</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
@@ -2090,24 +2090,24 @@
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>5677</t>
+          <t>5936</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>15035</t>
+          <t>10552</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>56133764</t>
+          <t>22885399</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>ustcarter</t>
+          <t>余文琪</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
@@ -2117,24 +2117,24 @@
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>5308</t>
+          <t>5857</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>16474</t>
+          <t>12006</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>6809364</t>
+          <t>37861953</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>"Scorp IP"</t>
+          <t>"Durex ๑• . •๑"</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
@@ -2144,24 +2144,24 @@
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>5219</t>
+          <t>5708</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>17019</t>
+          <t>12498</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>8057001</t>
+          <t>56133764</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>㊥兵者诡道也</t>
+          <t>ustcarter</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
@@ -2171,24 +2171,24 @@
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>5186</t>
+          <t>5660</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>18944</t>
+          <t>16264</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>38995116</t>
+          <t>8057001</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>"Ramesh Pavai Nam"</t>
+          <t>㊥兵者诡道也</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
@@ -2198,24 +2198,24 @@
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>5067</t>
+          <t>5362</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>21511</t>
+          <t>16874</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>54778421</t>
+          <t>6809364</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>Emma</t>
+          <t>"Scorp IP"</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
@@ -2225,24 +2225,24 @@
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>4918</t>
+          <t>5323</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>22179</t>
+          <t>18580</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>11582001</t>
+          <t>38995116</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>iMinatoX4</t>
+          <t>"Ramesh Pavai Nam"</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
@@ -2252,24 +2252,24 @@
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>4882</t>
+          <t>5222</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>24171</t>
+          <t>20219</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>54085771</t>
+          <t>54778421</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>㊥Matthieu</t>
+          <t>Emma</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
@@ -2279,24 +2279,24 @@
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>4781</t>
+          <t>5120</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>32885</t>
+          <t>23598</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>55860890</t>
+          <t>11582001</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>㊥Ethan</t>
+          <t>iMinatoX4</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
@@ -2306,24 +2306,24 @@
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>4381</t>
+          <t>4918</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>33123</t>
+          <t>26211</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>56573048</t>
+          <t>54085771</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>Xiaotian</t>
+          <t>㊥Matthieu</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
@@ -2333,24 +2333,24 @@
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>4370</t>
+          <t>4778</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>33981</t>
+          <t>28690</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>38561634</t>
+          <t>55860890</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>"Ambrose PT"</t>
+          <t>㊥Ethan</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
@@ -2360,24 +2360,24 @@
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>4328</t>
+          <t>4660</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>35986</t>
+          <t>30563</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>31401481</t>
+          <t>56573048</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>Player-31401481</t>
+          <t>Xiaotian</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
@@ -2387,24 +2387,24 @@
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>4232</t>
+          <t>4579</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>37449</t>
+          <t>31429</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>32316256</t>
+          <t>31401481</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>"秋の風 .."</t>
+          <t>Player-31401481</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
@@ -2414,24 +2414,24 @@
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>4166</t>
+          <t>4541</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>39740</t>
+          <t>32450</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>58203298</t>
+          <t>32316256</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>权旨qua</t>
+          <t>"秋の風 .."</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
@@ -2441,24 +2441,24 @@
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>4053</t>
+          <t>4492</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>40561</t>
+          <t>33192</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>56500325</t>
+          <t>38561634</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>haruharuyukizg9735</t>
+          <t>"Ambrose PT"</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
@@ -2468,14 +2468,14 @@
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>4009</t>
+          <t>4454</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>42223</t>
+          <t>36120</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
@@ -2495,14 +2495,14 @@
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>3914</t>
+          <t>4300</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>42965</t>
+          <t>40394</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -2522,24 +2522,24 @@
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>3839</t>
+          <t>4085</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>48522</t>
+          <t>40806</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>1550355</t>
+          <t>58203298</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>"皓茵 世界"</t>
+          <t>权旨qua</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
@@ -2549,24 +2549,24 @@
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>3332</t>
+          <t>4064</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>49969</t>
+          <t>41099</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>22161051</t>
+          <t>56500325</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>Botz5</t>
+          <t>haruharuyukizg9735</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
@@ -2576,24 +2576,24 @@
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>3229</t>
+          <t>4047</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>51559</t>
+          <t>49407</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>57813281</t>
+          <t>1550355</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>XAUEN</t>
+          <t>"皓茵 世界"</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
@@ -2603,24 +2603,24 @@
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>3111</t>
+          <t>3331</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>56814</t>
+          <t>50917</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>68132</t>
+          <t>22161051</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>"㊖TW9 百媚生"</t>
+          <t>Botz5</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
@@ -2630,24 +2630,24 @@
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>2849</t>
+          <t>3225</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>58989</t>
+          <t>52574</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>14110169</t>
+          <t>57813281</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>"Pasiony CANQ"</t>
+          <t>XAUEN</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
@@ -2657,24 +2657,24 @@
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>2758</t>
+          <t>3103</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>60905</t>
+          <t>56172</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>24733875</t>
+          <t>68132</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>龍少</t>
+          <t>"㊖TW9 百媚生"</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
@@ -2684,24 +2684,24 @@
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>2689</t>
+          <t>2912</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>999999</t>
+          <t>59688</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>29565</t>
+          <t>14110169</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>"aK.j Zhong ㊥"</t>
+          <t>"Pasiony CANQ"</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
@@ -2711,24 +2711,24 @@
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2758</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>999999</t>
+          <t>61645</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>12639656</t>
+          <t>24733875</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>"wu huang"</t>
+          <t>龍少</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
@@ -2738,7 +2738,7 @@
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2689</t>
         </is>
       </c>
     </row>
@@ -2750,12 +2750,12 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>47758619</t>
+          <t>29565</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>"㊥ Moon ㊥"</t>
+          <t>"aK.j Zhong ㊥"</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
@@ -2777,12 +2777,12 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>44789201</t>
+          <t>12639656</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>华夏四川广安</t>
+          <t>"wu huang"</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
@@ -2804,12 +2804,12 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>32478707</t>
+          <t>47758619</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>"Bt So"</t>
+          <t>"㊥ Moon ㊥"</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
@@ -2826,27 +2826,27 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>14811</t>
+          <t>999999</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>31134300</t>
+          <t>44789201</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>McMaX</t>
+          <t>华夏四川广安</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>二馆</t>
+          <t>一馆</t>
         </is>
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>5324</t>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -2858,17 +2858,17 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>44378757</t>
+          <t>32478707</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>"NᵉᵗʰᵉʳDʳⁱᶠᵗᵉʳ ㊥"</t>
+          <t>"Bt So"</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>二馆</t>
+          <t>一馆</t>
         </is>
       </c>
       <c r="E93" t="inlineStr">
@@ -2880,17 +2880,17 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>22386</t>
+          <t>15535</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>46289694</t>
+          <t>31134300</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>㊥Vincent</t>
+          <t>McMaX</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
@@ -2900,24 +2900,24 @@
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>4872</t>
+          <t>5411</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>22882</t>
+          <t>52015</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>37069173</t>
+          <t>43281368</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>詹toniii</t>
+          <t>xhs2763</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
@@ -2927,24 +2927,24 @@
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>4845</t>
+          <t>3140</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>24530</t>
+          <t>69416</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>25479797</t>
+          <t>44378757</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>"Mohamed Alnaqbi"</t>
+          <t>"NᵉᵗʰᵉʳDʳⁱᶠᵗᵉʳ ㊥"</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
@@ -2954,24 +2954,24 @@
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>4765</t>
+          <t>2500</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>25587</t>
+          <t>23272</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>28855852</t>
+          <t>25479797</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>tiger</t>
+          <t>"Mohamed Alnaqbi"</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
@@ -2981,24 +2981,24 @@
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>4715</t>
+          <t>4937</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>26739</t>
+          <t>24324</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>44708798</t>
+          <t>37069173</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>"㊥ mythgod"</t>
+          <t>詹toniii</t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
@@ -3008,24 +3008,24 @@
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>4659</t>
+          <t>4875</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>51944</t>
+          <t>26454</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>54588689</t>
+          <t>28855852</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>㊥墨衍枫迹☜</t>
+          <t>tiger</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
@@ -3035,24 +3035,24 @@
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>3087</t>
+          <t>4766</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>8244</t>
+          <t>26739</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>7025661</t>
+          <t>44708798</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>"F ᶻᵍˣ"</t>
+          <t>"㊥ mythgod"</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
@@ -3062,24 +3062,24 @@
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>5899</t>
+          <t>4752</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>11770</t>
+          <t>52653</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>25163202</t>
+          <t>54588689</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>"sam yang"</t>
+          <t>㊥墨衍枫迹☜</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
@@ -3089,24 +3089,24 @@
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>5560</t>
+          <t>3098</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>24401</t>
+          <t>8350</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>55634661</t>
+          <t>7025661</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>Opalus</t>
+          <t>"F ᶻᵍˣ"</t>
         </is>
       </c>
       <c r="D102" t="inlineStr">
@@ -3116,14 +3116,14 @@
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t>4770</t>
+          <t>6078</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>26433</t>
+          <t>22060</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
@@ -3143,24 +3143,24 @@
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>4674</t>
+          <t>5008</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>30195</t>
+          <t>26397</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>47459684</t>
+          <t>55634661</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>㊥阿闹切克闹</t>
+          <t>Opalus</t>
         </is>
       </c>
       <c r="D104" t="inlineStr">
@@ -3170,24 +3170,24 @@
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t>4509</t>
+          <t>4768</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>31244</t>
+          <t>29333</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>58743790</t>
+          <t>18082891</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>Ma</t>
+          <t>Michael</t>
         </is>
       </c>
       <c r="D105" t="inlineStr">
@@ -3197,24 +3197,24 @@
       </c>
       <c r="E105" t="inlineStr">
         <is>
-          <t>4461</t>
+          <t>4632</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>33101</t>
+          <t>30675</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>56585361</t>
+          <t>47459684</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>"㊥ go策划我要ali"</t>
+          <t>㊥阿闹切克闹</t>
         </is>
       </c>
       <c r="D106" t="inlineStr">
@@ -3224,24 +3224,24 @@
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t>4371</t>
+          <t>4575</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>33281</t>
+          <t>31866</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>56379103</t>
+          <t>3649043</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>Globalking</t>
+          <t>Dj6106</t>
         </is>
       </c>
       <c r="D107" t="inlineStr">
@@ -3251,24 +3251,24 @@
       </c>
       <c r="E107" t="inlineStr">
         <is>
-          <t>4362</t>
+          <t>4520</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>33294</t>
+          <t>32962</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>3649043</t>
+          <t>58743790</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>Dj6106</t>
+          <t>Ma</t>
         </is>
       </c>
       <c r="D108" t="inlineStr">
@@ -3278,24 +3278,24 @@
       </c>
       <c r="E108" t="inlineStr">
         <is>
-          <t>4362</t>
+          <t>4466</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>34229</t>
+          <t>34144</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>18082891</t>
+          <t>56379103</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>Michael</t>
+          <t>Globalking</t>
         </is>
       </c>
       <c r="D109" t="inlineStr">
@@ -3305,14 +3305,14 @@
       </c>
       <c r="E109" t="inlineStr">
         <is>
-          <t>4317</t>
+          <t>4402</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>34906</t>
+          <t>34344</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
@@ -3332,24 +3332,24 @@
       </c>
       <c r="E110" t="inlineStr">
         <is>
-          <t>4282</t>
+          <t>4392</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>35537</t>
+          <t>36406</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>58839983</t>
+          <t>55499394</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>每逢佳节胖六斤</t>
+          <t>Player-55499394</t>
         </is>
       </c>
       <c r="D111" t="inlineStr">
@@ -3359,24 +3359,24 @@
       </c>
       <c r="E111" t="inlineStr">
         <is>
-          <t>4251</t>
+          <t>4285</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>36007</t>
+          <t>36466</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>55499394</t>
+          <t>56585361</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>Player-55499394</t>
+          <t>"㊥ go策划我要ali"</t>
         </is>
       </c>
       <c r="D112" t="inlineStr">
@@ -3386,24 +3386,24 @@
       </c>
       <c r="E112" t="inlineStr">
         <is>
-          <t>4231</t>
+          <t>4282</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>38763</t>
+          <t>37023</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>58408326</t>
+          <t>58839983</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>"Killer Bee"</t>
+          <t>每逢佳节胖六斤</t>
         </is>
       </c>
       <c r="D113" t="inlineStr">
@@ -3413,14 +3413,14 @@
       </c>
       <c r="E113" t="inlineStr">
         <is>
-          <t>4101</t>
+          <t>4254</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>39453</t>
+          <t>39783</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
@@ -3440,24 +3440,24 @@
       </c>
       <c r="E114" t="inlineStr">
         <is>
-          <t>4068</t>
+          <t>4116</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>40378</t>
+          <t>40676</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>47244896</t>
+          <t>58408326</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>Dropthebeat</t>
+          <t>"Killer Bee"</t>
         </is>
       </c>
       <c r="D115" t="inlineStr">
@@ -3467,14 +3467,14 @@
       </c>
       <c r="E115" t="inlineStr">
         <is>
-          <t>4020</t>
+          <t>4071</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>40432</t>
+          <t>41462</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
@@ -3494,24 +3494,24 @@
       </c>
       <c r="E116" t="inlineStr">
         <is>
-          <t>4017</t>
+          <t>4026</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>42201</t>
+          <t>41526</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>48738257</t>
+          <t>47244896</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>死亡洲际跳蛋</t>
+          <t>Dropthebeat</t>
         </is>
       </c>
       <c r="D117" t="inlineStr">
@@ -3521,24 +3521,24 @@
       </c>
       <c r="E117" t="inlineStr">
         <is>
-          <t>3916</t>
+          <t>4021</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>44176</t>
+          <t>43017</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>52997727</t>
+          <t>48738257</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>larios</t>
+          <t>死亡洲际跳蛋</t>
         </is>
       </c>
       <c r="D118" t="inlineStr">
@@ -3548,14 +3548,14 @@
       </c>
       <c r="E118" t="inlineStr">
         <is>
-          <t>3716</t>
+          <t>3939</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>44201</t>
+          <t>43541</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
@@ -3575,24 +3575,24 @@
       </c>
       <c r="E119" t="inlineStr">
         <is>
-          <t>3715</t>
+          <t>3892</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>44711</t>
+          <t>43656</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>58641574</t>
+          <t>52997727</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>Player-58641574鱼</t>
+          <t>larios</t>
         </is>
       </c>
       <c r="D120" t="inlineStr">
@@ -3602,24 +3602,24 @@
       </c>
       <c r="E120" t="inlineStr">
         <is>
-          <t>3666</t>
+          <t>3880</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>46046</t>
+          <t>45798</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>48634530</t>
+          <t>58641574</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>leezhenrui</t>
+          <t>Player-58641574鱼</t>
         </is>
       </c>
       <c r="D121" t="inlineStr">
@@ -3629,24 +3629,24 @@
       </c>
       <c r="E121" t="inlineStr">
         <is>
-          <t>3542</t>
+          <t>3655</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>47090</t>
+          <t>46442</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>56700848</t>
+          <t>48634530</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>工口漫画老师</t>
+          <t>leezhenrui</t>
         </is>
       </c>
       <c r="D122" t="inlineStr">
@@ -3656,24 +3656,24 @@
       </c>
       <c r="E122" t="inlineStr">
         <is>
-          <t>3453</t>
+          <t>3591</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>49093</t>
+          <t>48002</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>58940575</t>
+          <t>56700848</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>图啊图z z</t>
+          <t>工口漫画老师</t>
         </is>
       </c>
       <c r="D123" t="inlineStr">
@@ -3683,24 +3683,24 @@
       </c>
       <c r="E123" t="inlineStr">
         <is>
-          <t>3288</t>
+          <t>3450</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>51047</t>
+          <t>50384</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>52157846</t>
+          <t>58940575</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>Hamza</t>
+          <t>图啊图z z</t>
         </is>
       </c>
       <c r="D124" t="inlineStr">
@@ -3710,24 +3710,24 @@
       </c>
       <c r="E124" t="inlineStr">
         <is>
-          <t>3147</t>
+          <t>3260</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>51304</t>
+          <t>52075</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>43281368</t>
+          <t>52157846</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>xhs2763</t>
+          <t>Hamza</t>
         </is>
       </c>
       <c r="D125" t="inlineStr">
@@ -3737,24 +3737,24 @@
       </c>
       <c r="E125" t="inlineStr">
         <is>
-          <t>3130</t>
+          <t>3136</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>62095</t>
+          <t>61847</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>47430231</t>
+          <t>52792063</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>Kentantrino</t>
+          <t>"Tramaine Dowlen"</t>
         </is>
       </c>
       <c r="D126" t="inlineStr">
@@ -3764,24 +3764,24 @@
       </c>
       <c r="E126" t="inlineStr">
         <is>
-          <t>2651</t>
+          <t>2682</t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>62184</t>
+          <t>63043</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>5367482</t>
+          <t>47430231</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>Ігор</t>
+          <t>Kentantrino</t>
         </is>
       </c>
       <c r="D127" t="inlineStr">
@@ -3791,24 +3791,24 @@
       </c>
       <c r="E127" t="inlineStr">
         <is>
-          <t>2648</t>
+          <t>2645</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>63101</t>
+          <t>63103</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>52792063</t>
+          <t>5367482</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>"Tramaine Dowlen"</t>
+          <t>Ігор</t>
         </is>
       </c>
       <c r="D128" t="inlineStr">
@@ -3818,14 +3818,14 @@
       </c>
       <c r="E128" t="inlineStr">
         <is>
-          <t>2621</t>
+          <t>2643</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>63575</t>
+          <t>63370</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
@@ -3845,14 +3845,14 @@
       </c>
       <c r="E129" t="inlineStr">
         <is>
-          <t>2608</t>
+          <t>2635</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>63870</t>
+          <t>63603</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
@@ -3872,14 +3872,14 @@
       </c>
       <c r="E130" t="inlineStr">
         <is>
-          <t>2600</t>
+          <t>2628</t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>71071</t>
+          <t>71446</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
@@ -3899,14 +3899,14 @@
       </c>
       <c r="E131" t="inlineStr">
         <is>
-          <t>2456</t>
+          <t>2467</t>
         </is>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>72895</t>
+          <t>73387</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
@@ -3926,14 +3926,14 @@
       </c>
       <c r="E132" t="inlineStr">
         <is>
-          <t>2385</t>
+          <t>2398</t>
         </is>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>89096</t>
+          <t>90354</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
@@ -3953,14 +3953,14 @@
       </c>
       <c r="E133" t="inlineStr">
         <is>
-          <t>2004</t>
+          <t>1999</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>94734</t>
+          <t>95800</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
@@ -3980,14 +3980,14 @@
       </c>
       <c r="E134" t="inlineStr">
         <is>
-          <t>1779</t>
+          <t>1782</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>147811</t>
+          <t>151043</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
@@ -4007,7 +4007,7 @@
       </c>
       <c r="E135" t="inlineStr">
         <is>
-          <t>1126</t>
+          <t>1125</t>
         </is>
       </c>
     </row>
@@ -4176,7 +4176,7 @@
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>51193</t>
+          <t>51875</t>
         </is>
       </c>
       <c r="B142" t="inlineStr">
@@ -4196,14 +4196,14 @@
       </c>
       <c r="E142" t="inlineStr">
         <is>
-          <t>3137</t>
+          <t>3150</t>
         </is>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>43530</t>
+          <t>44785</t>
         </is>
       </c>
       <c r="B143" t="inlineStr">
@@ -4223,7 +4223,7 @@
       </c>
       <c r="E143" t="inlineStr">
         <is>
-          <t>3782</t>
+          <t>3757</t>
         </is>
       </c>
     </row>
@@ -4257,7 +4257,7 @@
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>49828</t>
+          <t>50334</t>
         </is>
       </c>
       <c r="B145" t="inlineStr">
@@ -4277,7 +4277,7 @@
       </c>
       <c r="E145" t="inlineStr">
         <is>
-          <t>3237</t>
+          <t>3264</t>
         </is>
       </c>
     </row>
@@ -4311,7 +4311,7 @@
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>81755</t>
+          <t>82225</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
@@ -4331,14 +4331,14 @@
       </c>
       <c r="E147" t="inlineStr">
         <is>
-          <t>2166</t>
+          <t>2180</t>
         </is>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>91926</t>
+          <t>92616</t>
         </is>
       </c>
       <c r="B148" t="inlineStr">
@@ -4358,24 +4358,24 @@
       </c>
       <c r="E148" t="inlineStr">
         <is>
-          <t>1896</t>
+          <t>1911</t>
         </is>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>113678</t>
+          <t>105603</t>
         </is>
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>41231396</t>
+          <t>59082827</t>
         </is>
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>ollsthebro</t>
+          <t>Player-59082827</t>
         </is>
       </c>
       <c r="D149" t="inlineStr">
@@ -4385,24 +4385,24 @@
       </c>
       <c r="E149" t="inlineStr">
         <is>
-          <t>1498</t>
+          <t>1586</t>
         </is>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>999999</t>
+          <t>115172</t>
         </is>
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>58572199</t>
+          <t>41231396</t>
         </is>
       </c>
       <c r="C150" t="inlineStr">
         <is>
-          <t>你干嘛～哎呦～</t>
+          <t>ollsthebro</t>
         </is>
       </c>
       <c r="D150" t="inlineStr">
@@ -4412,7 +4412,7 @@
       </c>
       <c r="E150" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1498</t>
         </is>
       </c>
     </row>
@@ -4424,12 +4424,12 @@
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>58766144</t>
+          <t>58572199</t>
         </is>
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>EquablePrecedence38</t>
+          <t>你干嘛～哎呦～</t>
         </is>
       </c>
       <c r="D151" t="inlineStr">
@@ -4451,12 +4451,12 @@
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>29355299</t>
+          <t>58766144</t>
         </is>
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>Player-29355299</t>
+          <t>EquablePrecedence38</t>
         </is>
       </c>
       <c r="D152" t="inlineStr">
@@ -4478,12 +4478,12 @@
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>58910668</t>
+          <t>29355299</t>
         </is>
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>BrittleAuthor33</t>
+          <t>Player-29355299</t>
         </is>
       </c>
       <c r="D153" t="inlineStr">
@@ -4505,12 +4505,12 @@
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>55745105</t>
+          <t>58910668</t>
         </is>
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>eldeniz</t>
+          <t>BrittleAuthor33</t>
         </is>
       </c>
       <c r="D154" t="inlineStr">
@@ -4532,12 +4532,12 @@
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>58174442</t>
+          <t>55745105</t>
         </is>
       </c>
       <c r="C155" t="inlineStr">
         <is>
-          <t>Player-58174442</t>
+          <t>eldeniz</t>
         </is>
       </c>
       <c r="D155" t="inlineStr">
@@ -4554,44 +4554,44 @@
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>54780</t>
+          <t>999999</t>
         </is>
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>10636651</t>
+          <t>58174442</t>
         </is>
       </c>
       <c r="C156" t="inlineStr">
         <is>
-          <t>"Ismail Aflou"</t>
+          <t>Player-58174442</t>
         </is>
       </c>
       <c r="D156" t="inlineStr">
         <is>
-          <t>Chinese</t>
+          <t>三馆</t>
         </is>
       </c>
       <c r="E156" t="inlineStr">
         <is>
-          <t>2940</t>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>50497</t>
+          <t>55593</t>
         </is>
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>41848598</t>
+          <t>10636651</t>
         </is>
       </c>
       <c r="C157" t="inlineStr">
         <is>
-          <t>国家一级保护沙雕</t>
+          <t>"Ismail Aflou"</t>
         </is>
       </c>
       <c r="D157" t="inlineStr">
@@ -4601,24 +4601,24 @@
       </c>
       <c r="E157" t="inlineStr">
         <is>
-          <t>3189</t>
+          <t>2940</t>
         </is>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>63692</t>
+          <t>50570</t>
         </is>
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>6010122</t>
+          <t>41848598</t>
         </is>
       </c>
       <c r="C158" t="inlineStr">
         <is>
-          <t>"Edward Peng"</t>
+          <t>国家一级保护沙雕</t>
         </is>
       </c>
       <c r="D158" t="inlineStr">
@@ -4628,24 +4628,24 @@
       </c>
       <c r="E158" t="inlineStr">
         <is>
-          <t>2604</t>
+          <t>3248</t>
         </is>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>999999</t>
+          <t>64409</t>
         </is>
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>12648101</t>
+          <t>6010122</t>
         </is>
       </c>
       <c r="C159" t="inlineStr">
         <is>
-          <t>"player 198827"</t>
+          <t>"Edward Peng"</t>
         </is>
       </c>
       <c r="D159" t="inlineStr">
@@ -4655,7 +4655,7 @@
       </c>
       <c r="E159" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2604</t>
         </is>
       </c>
     </row>
@@ -4667,12 +4667,12 @@
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>9195340</t>
+          <t>12648101</t>
         </is>
       </c>
       <c r="C160" t="inlineStr">
         <is>
-          <t>Namllllllik</t>
+          <t>"player 198827"</t>
         </is>
       </c>
       <c r="D160" t="inlineStr">
@@ -4694,12 +4694,12 @@
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>15755724</t>
+          <t>9195340</t>
         </is>
       </c>
       <c r="C161" t="inlineStr">
         <is>
-          <t>"Last Good"</t>
+          <t>Namllllllik</t>
         </is>
       </c>
       <c r="D161" t="inlineStr">
@@ -4721,12 +4721,12 @@
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>8850180</t>
+          <t>15755724</t>
         </is>
       </c>
       <c r="C162" t="inlineStr">
         <is>
-          <t>30624300</t>
+          <t>"Last Good"</t>
         </is>
       </c>
       <c r="D162" t="inlineStr">
@@ -4748,12 +4748,12 @@
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>28624723</t>
+          <t>8850180</t>
         </is>
       </c>
       <c r="C163" t="inlineStr">
         <is>
-          <t>"Woody Shade"</t>
+          <t>30624300</t>
         </is>
       </c>
       <c r="D163" t="inlineStr">
@@ -4775,20 +4775,47 @@
       </c>
       <c r="B164" t="inlineStr">
         <is>
+          <t>28624723</t>
+        </is>
+      </c>
+      <c r="C164" t="inlineStr">
+        <is>
+          <t>"Woody Shade"</t>
+        </is>
+      </c>
+      <c r="D164" t="inlineStr">
+        <is>
+          <t>Chinese</t>
+        </is>
+      </c>
+      <c r="E164" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="inlineStr">
+        <is>
+          <t>999999</t>
+        </is>
+      </c>
+      <c r="B165" t="inlineStr">
+        <is>
           <t>9913517</t>
         </is>
       </c>
-      <c r="C164" t="inlineStr">
+      <c r="C165" t="inlineStr">
         <is>
           <t>"Kenny Chan"</t>
         </is>
       </c>
-      <c r="D164" t="inlineStr">
+      <c r="D165" t="inlineStr">
         <is>
           <t>Chinese</t>
         </is>
       </c>
-      <c r="E164" t="inlineStr">
+      <c r="E165" t="inlineStr">
         <is>
           <t>0</t>
         </is>

</xml_diff>

<commit_message>
Code updated 23-03-26 08:37:20
</commit_message>
<xml_diff>
--- a/Season_Trophies/86.xlsx
+++ b/Season_Trophies/86.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E165"/>
+  <dimension ref="A1:E158"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -396,7 +396,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>45710</t>
+          <t>46192</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -423,17 +423,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>455</t>
+          <t>251</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>32613475</t>
+          <t>26424998</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>"李 无 善 德"</t>
+          <t>"Smok3y 1nOnly"</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -443,24 +443,24 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>7481</t>
+          <t>7573</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>705</t>
+          <t>485</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>6940556</t>
+          <t>32613475</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>"Cry ab it林黛玉ᶻᵍˣ"</t>
+          <t>"李 无 善 德"</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -470,24 +470,24 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>7385</t>
+          <t>7472</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>925</t>
+          <t>731</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>26424998</t>
+          <t>6940556</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>"Smok3y 1nOnly"</t>
+          <t>"Cry ab it林黛玉ᶻᵍˣ"</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -497,14 +497,14 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>7318</t>
+          <t>7383</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>3158</t>
+          <t>3367</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -531,7 +531,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>9615</t>
+          <t>5892</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -551,14 +551,14 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>5955</t>
+          <t>6415</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>214</t>
+          <t>209</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -585,17 +585,17 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>1160</t>
+          <t>768</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>27468237</t>
+          <t>3946814</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>佛系复仇者秀川</t>
+          <t>"小瑩 潘"</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -605,24 +605,24 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>7252</t>
+          <t>7371</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>1367</t>
+          <t>1216</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>3946814</t>
+          <t>27468237</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>"小瑩 潘"</t>
+          <t>佛系复仇者秀川</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -632,14 +632,14 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>7192</t>
+          <t>7257</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2955</t>
+          <t>2076</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -659,14 +659,14 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>6858</t>
+          <t>7062</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>8883</t>
+          <t>9329</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -686,14 +686,14 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>6028</t>
+          <t>6027</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>9742</t>
+          <t>10055</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -713,24 +713,24 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>5942</t>
+          <t>5957</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>11270</t>
+          <t>10251</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>21665473</t>
+          <t>14424176</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>"Dog Gamedesiger"</t>
+          <t>天才少年老纪</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -740,24 +740,24 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>5785</t>
+          <t>5937</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>12520</t>
+          <t>11723</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>14424176</t>
+          <t>21665473</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>天才少年老纪</t>
+          <t>"Dog Gamedesiger"</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -767,14 +767,14 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>5659</t>
+          <t>5785</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>166</t>
+          <t>183</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -794,24 +794,24 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>7607</t>
+          <t>7601</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>1912</t>
+          <t>800</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>31267627</t>
+          <t>1951758</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>"㊥ Martin"</t>
+          <t>我來找你了</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -821,24 +821,24 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>7060</t>
+          <t>7362</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2240</t>
+          <t>1307</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>25376635</t>
+          <t>8741713</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>"sanchez ᶻᵍˣ"</t>
+          <t xml:space="preserve">㊥大咖玩家ky </t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -848,24 +848,24 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>6997</t>
+          <t>7232</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2403</t>
+          <t>1856</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>1820342</t>
+          <t>29211638</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>摸鱼爱好者三战</t>
+          <t>"㊥ PhononDisperse"</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -875,24 +875,24 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>6961</t>
+          <t>7103</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2464</t>
+          <t>2080</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>46422609</t>
+          <t>31267627</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>㊥林天大大神</t>
+          <t>"㊥ Martin"</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -902,24 +902,24 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>6947</t>
+          <t>7060</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>3152</t>
+          <t>2218</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>11783968</t>
+          <t>25376635</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>F---119</t>
+          <t>"sanchez ᶻᵍˣ"</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -929,24 +929,24 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>6818</t>
+          <t>7033</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>4080</t>
+          <t>2308</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>3477306</t>
+          <t>1820342</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>"MeGa Tsai"</t>
+          <t>摸鱼爱好者三战</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -956,24 +956,24 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>6647</t>
+          <t>7017</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>4477</t>
+          <t>2859</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>21735478</t>
+          <t>46422609</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>耀翔fly</t>
+          <t>㊥林天大大神</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -983,24 +983,24 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>6585</t>
+          <t>6909</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>5055</t>
+          <t>3276</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>26280580</t>
+          <t>31217211</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>AOW全体工作人员吃屎交易大厅</t>
+          <t>解憂雜貨鋪㊥</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -1010,24 +1010,24 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>6491</t>
+          <t>6833</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>5165</t>
+          <t>3363</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>30411791</t>
+          <t>11783968</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>"㊥Ⓩ GOÐAFRÆÐI ᶻᵍˣ"</t>
+          <t>F---119</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -1037,24 +1037,24 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>6476</t>
+          <t>6818</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>5252</t>
+          <t>3386</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>33656016</t>
+          <t>28749280</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>㊥☆梅海听雪☆</t>
+          <t>㊥老船⛵⛵</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -1064,24 +1064,24 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>6461</t>
+          <t>6813</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>5312</t>
+          <t>3729</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>28749280</t>
+          <t>16206490</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>㊥老船⛵⛵</t>
+          <t>㊥Godcys</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -1091,24 +1091,24 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>6452</t>
+          <t>6752</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>5464</t>
+          <t>4189</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>38711610</t>
+          <t>21735478</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>心灵有为</t>
+          <t>耀翔fly</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -1118,24 +1118,24 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>6429</t>
+          <t>6670</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>5594</t>
+          <t>4263</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>6510348</t>
+          <t>3477306</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Bonpoisson</t>
+          <t>"MeGa Tsai"</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -1145,24 +1145,24 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>6414</t>
+          <t>6658</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>5158</t>
+          <t>4080</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>9541747</t>
+          <t>26280580</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>豹子头林冲</t>
+          <t>AOW全体工作人员吃屎交易大厅</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -1172,24 +1172,24 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>6476</t>
+          <t>6692</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>6665</t>
+          <t>5274</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>31217211</t>
+          <t>30411791</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>解憂雜貨鋪㊥</t>
+          <t>"㊥Ⓩ GOÐAFRÆÐI ᶻᵍˣ"</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -1199,24 +1199,24 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>6276</t>
+          <t>6501</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>7458</t>
+          <t>5544</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>29729468</t>
+          <t>9541747</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>"风神舞动 WDᶻᵍˣ"</t>
+          <t>豹子头林冲</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -1226,24 +1226,24 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>6179</t>
+          <t>6463</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>8301</t>
+          <t>5647</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>44955827</t>
+          <t>38711610</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>丶小阿狸丿</t>
+          <t>心灵有为</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -1253,24 +1253,24 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>6083</t>
+          <t>6446</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>13190</t>
+          <t>5737</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>47146736</t>
+          <t>33656016</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>"HK 品瑜"</t>
+          <t>㊥☆梅海听雪☆</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -1280,24 +1280,24 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>5595</t>
+          <t>6433</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>14118</t>
+          <t>6290</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>12333251</t>
+          <t>6510348</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>"㊌ Mingxuan"</t>
+          <t>Bonpoisson</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
@@ -1307,24 +1307,24 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>5515</t>
+          <t>6365</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>16054</t>
+          <t>7919</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>29861826</t>
+          <t>29729468</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>★★★Eric★★★</t>
+          <t>"风神舞动 WDᶻᵍˣ"</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -1334,24 +1334,24 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>5375</t>
+          <t>6170</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>17507</t>
+          <t>8754</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>55317038</t>
+          <t>7025661</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>necman12345</t>
+          <t>"F ᶻᵍˣ"</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -1361,24 +1361,24 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>5288</t>
+          <t>6078</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>21724</t>
+          <t>9098</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>45967307</t>
+          <t>44955827</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Ricky</t>
+          <t>丶小阿狸丿</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -1388,24 +1388,24 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>5027</t>
+          <t>6047</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>23366</t>
+          <t>12171</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>20737010</t>
+          <t>47146736</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>混着玩...</t>
+          <t>"HK 品瑜"</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
@@ -1415,24 +1415,24 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>4932</t>
+          <t>5740</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>24796</t>
+          <t>13763</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>46289694</t>
+          <t>12333251</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>㊥Vincent</t>
+          <t>"㊌ Mingxuan"</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
@@ -1442,24 +1442,24 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>4849</t>
+          <t>5596</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>26409</t>
+          <t>16834</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>32929656</t>
+          <t>29861826</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>"EIH Wilson Chu"</t>
+          <t>★★★Eric★★★</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -1469,24 +1469,24 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>4768</t>
+          <t>5375</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>49331</t>
+          <t>18442</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>7587898</t>
+          <t>55317038</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>藍精靈ᶻᵍˣ</t>
+          <t>necman12345</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
@@ -1496,24 +1496,24 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>3336</t>
+          <t>5283</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>66757</t>
+          <t>18506</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>47928278</t>
+          <t>28387448</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>"落日幻影 哈哈哈"</t>
+          <t>☜⊙‖⊙☞</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
@@ -1523,24 +1523,24 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>2548</t>
+          <t>5280</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>999999</t>
+          <t>18150</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>23687250</t>
+          <t>45967307</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>"jetlijp ᶻᵍˣ"</t>
+          <t>Ricky</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
@@ -1550,159 +1550,159 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>5300</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>2780</t>
+          <t>23963</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>27484940</t>
+          <t>46289694</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>66666zgx</t>
+          <t>㊥Vincent</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>一馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>6888</t>
+          <t>4948</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>19258</t>
+          <t>24234</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>38809086</t>
+          <t>20737010</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Kouenᶻᵍˣ</t>
+          <t>混着玩...</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>一馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>5184</t>
+          <t>4932</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>6223</t>
+          <t>49457</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>13738844</t>
+          <t>7587898</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>"Chen Hao"</t>
+          <t>藍精靈ᶻᵍˣ</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>一馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>6333</t>
+          <t>3368</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>9262</t>
+          <t>67172</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>42434117</t>
+          <t>47928278</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>㊥有双飞鸟</t>
+          <t>"落日幻影 哈哈哈"</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>一馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>5998</t>
+          <t>2548</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>11780</t>
+          <t>999999</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>53060417</t>
+          <t>23687250</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>㊥老纳信耶稣</t>
+          <t>"jetlijp ᶻᵍˣ"</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>一馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>5732</t>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>12413</t>
+          <t>4724</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>49710892</t>
+          <t>26588375</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>MMMMMMM</t>
+          <t>何苦僧ai</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
@@ -1712,24 +1712,24 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>5668</t>
+          <t>6585</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>12888</t>
+          <t>6581</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>53520939</t>
+          <t>13738844</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>㊥虎哥tiger</t>
+          <t>"Chen Hao"</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
@@ -1739,24 +1739,24 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>5623</t>
+          <t>6330</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>15808</t>
+          <t>12173</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>31495601</t>
+          <t>37861953</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>陈晓军</t>
+          <t>"Durex ๑• . •๑"</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
@@ -1766,24 +1766,24 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>5392</t>
+          <t>5740</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>17343</t>
+          <t>18596</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>54698813</t>
+          <t>38809086</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>閃亮唐老鴨</t>
+          <t>Kouenᶻᵍˣ</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
@@ -1793,24 +1793,24 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>5298</t>
+          <t>5275</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>18873</t>
+          <t>10104</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>4756174</t>
+          <t>42434117</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>純希です</t>
+          <t>㊥有双飞鸟</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
@@ -1820,24 +1820,24 @@
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>5206</t>
+          <t>5952</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>23344</t>
+          <t>10814</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>55769051</t>
+          <t>49710892</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>㊥叮叮当.</t>
+          <t>MMMMMMM</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
@@ -1847,24 +1847,24 @@
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>4932</t>
+          <t>5873</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>999999</t>
+          <t>13081</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>43812707</t>
+          <t>53060417</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>bbtt</t>
+          <t>㊥老纳信耶稣</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
@@ -1874,24 +1874,24 @@
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>5653</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>1109</t>
+          <t>13066</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>1951758</t>
+          <t>53520939</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>我來找你了</t>
+          <t>㊥虎哥tiger</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
@@ -1901,24 +1901,24 @@
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>7267</t>
+          <t>5654</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>1144</t>
+          <t>15328</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>8741713</t>
+          <t>31495601</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t xml:space="preserve">㊥大咖玩家ky </t>
+          <t>陈晓军</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
@@ -1928,24 +1928,24 @@
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>7257</t>
+          <t>5474</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>1671</t>
+          <t>18034</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>29211638</t>
+          <t>4756174</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>"㊥ PhononDisperse"</t>
+          <t>純希です</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
@@ -1955,24 +1955,24 @@
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>7117</t>
+          <t>5305</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>4341</t>
+          <t>18552</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>26588375</t>
+          <t>54698813</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>何苦僧ai</t>
+          <t>閃亮唐老鴨</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
@@ -1982,24 +1982,24 @@
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>6603</t>
+          <t>5277</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>4418</t>
+          <t>24136</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>16206490</t>
+          <t>55769051</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>㊥Godcys</t>
+          <t>㊥叮叮当.</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
@@ -2009,14 +2009,14 @@
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>6591</t>
+          <t>4938</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>6811</t>
+          <t>7255</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
@@ -2036,14 +2036,14 @@
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>6258</t>
+          <t>6244</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>7547</t>
+          <t>7932</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
@@ -2070,7 +2070,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>9801</t>
+          <t>9747</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
@@ -2090,14 +2090,14 @@
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>5936</t>
+          <t>5996</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>10552</t>
+          <t>10990</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -2124,17 +2124,17 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>12006</t>
+          <t>15443</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>37861953</t>
+          <t>56133764</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>"Durex ๑• . •๑"</t>
+          <t>ustcarter</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
@@ -2144,24 +2144,24 @@
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>5708</t>
+          <t>5465</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>12498</t>
+          <t>16280</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>56133764</t>
+          <t>6809364</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>ustcarter</t>
+          <t>"Scorp IP"</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
@@ -2171,14 +2171,14 @@
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>5660</t>
+          <t>5410</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>16264</t>
+          <t>17304</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
@@ -2198,24 +2198,24 @@
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>5362</t>
+          <t>5346</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>16874</t>
+          <t>20251</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>6809364</t>
+          <t>38995116</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>"Scorp IP"</t>
+          <t>"Ramesh Pavai Nam"</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
@@ -2225,24 +2225,24 @@
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>5323</t>
+          <t>5172</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>18580</t>
+          <t>21663</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>38995116</t>
+          <t>54778421</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>"Ramesh Pavai Nam"</t>
+          <t>Emma</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
@@ -2252,24 +2252,24 @@
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>5222</t>
+          <t>5083</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>20219</t>
+          <t>24470</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>54778421</t>
+          <t>11582001</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>Emma</t>
+          <t>iMinatoX4</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
@@ -2279,24 +2279,24 @@
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>5120</t>
+          <t>4918</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>23598</t>
+          <t>25589</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>11582001</t>
+          <t>54085771</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>iMinatoX4</t>
+          <t>㊥Matthieu</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
@@ -2306,24 +2306,24 @@
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>4918</t>
+          <t>4856</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>26211</t>
+          <t>26039</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>54085771</t>
+          <t>32316256</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>㊥Matthieu</t>
+          <t>"秋の風 .."</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
@@ -2333,14 +2333,14 @@
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>4778</t>
+          <t>4834</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>28690</t>
+          <t>27262</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
@@ -2360,24 +2360,24 @@
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>4660</t>
+          <t>4773</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>30563</t>
+          <t>30456</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>56573048</t>
+          <t>38893233</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>Xiaotian</t>
+          <t>"快乐 二哈"</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
@@ -2387,24 +2387,24 @@
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>4579</t>
+          <t>4625</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>31429</t>
+          <t>32623</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>31401481</t>
+          <t>38561634</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>Player-31401481</t>
+          <t>"Ambrose PT"</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
@@ -2414,24 +2414,24 @@
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>4541</t>
+          <t>4530</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>32450</t>
+          <t>32650</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>32316256</t>
+          <t>31401481</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>"秋の風 .."</t>
+          <t>Player-31401481</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
@@ -2441,24 +2441,24 @@
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>4492</t>
+          <t>4529</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>33192</t>
+          <t>33146</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>38561634</t>
+          <t>56573048</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>"Ambrose PT"</t>
+          <t>Xiaotian</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
@@ -2468,24 +2468,24 @@
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>4454</t>
+          <t>4505</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>36120</t>
+          <t>40264</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>38893233</t>
+          <t>58203298</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>"快乐 二哈"</t>
+          <t>权旨qua</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
@@ -2495,14 +2495,14 @@
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>4300</t>
+          <t>4128</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>40394</t>
+          <t>41546</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -2522,24 +2522,24 @@
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>4085</t>
+          <t>4059</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>40806</t>
+          <t>42391</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>58203298</t>
+          <t>56500325</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>权旨qua</t>
+          <t>haruharuyukizg9735</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
@@ -2549,24 +2549,24 @@
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>4064</t>
+          <t>4007</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>41099</t>
+          <t>49430</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>56500325</t>
+          <t>57813281</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>haruharuyukizg9735</t>
+          <t>XAUEN</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
@@ -2576,14 +2576,14 @@
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>4047</t>
+          <t>3370</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>49407</t>
+          <t>49931</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
@@ -2603,14 +2603,14 @@
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>3331</t>
+          <t>3330</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>50917</t>
+          <t>51434</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
@@ -2630,24 +2630,24 @@
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>3225</t>
+          <t>3221</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>52574</t>
+          <t>55918</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>57813281</t>
+          <t>68132</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>XAUEN</t>
+          <t>"㊖TW9 百媚生"</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
@@ -2657,24 +2657,24 @@
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>3103</t>
+          <t>2943</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>56172</t>
+          <t>56551</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>68132</t>
+          <t>14110169</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>"㊖TW9 百媚生"</t>
+          <t>"Pasiony CANQ"</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
@@ -2684,24 +2684,24 @@
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>2912</t>
+          <t>2915</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>59688</t>
+          <t>62079</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>14110169</t>
+          <t>24733875</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>"Pasiony CANQ"</t>
+          <t>龍少</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
@@ -2711,24 +2711,24 @@
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>2758</t>
+          <t>2689</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>61645</t>
+          <t>70163</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>24733875</t>
+          <t>29565</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>龍少</t>
+          <t>"aK.j Zhong ㊥"</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
@@ -2738,7 +2738,7 @@
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>2689</t>
+          <t>2499</t>
         </is>
       </c>
     </row>
@@ -2750,12 +2750,12 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>29565</t>
+          <t>47758619</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>"aK.j Zhong ㊥"</t>
+          <t>"㊥ Moon ㊥"</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
@@ -2772,125 +2772,125 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>999999</t>
+          <t>16276</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>12639656</t>
+          <t>31134300</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>"wu huang"</t>
+          <t>McMaX</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>一馆</t>
+          <t>二馆</t>
         </is>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>5411</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>999999</t>
+          <t>43396</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>47758619</t>
+          <t>48738257</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>"㊥ Moon ㊥"</t>
+          <t>死亡洲际跳蛋</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>一馆</t>
+          <t>二馆</t>
         </is>
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>3953</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>999999</t>
+          <t>52447</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>44789201</t>
+          <t>43281368</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>华夏四川广安</t>
+          <t>xhs2763</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>一馆</t>
+          <t>二馆</t>
         </is>
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>3139</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>999999</t>
+          <t>69870</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>32478707</t>
+          <t>44378757</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>"Bt So"</t>
+          <t>"NᵉᵗʰᵉʳDʳⁱᶠᵗᵉʳ ㊥"</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>一馆</t>
+          <t>二馆</t>
         </is>
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2500</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>15535</t>
+          <t>22570</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>31134300</t>
+          <t>37069173</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>McMaX</t>
+          <t>詹toniii</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
@@ -2900,24 +2900,24 @@
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>5411</t>
+          <t>5028</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>52015</t>
+          <t>24158</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>43281368</t>
+          <t>25479797</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>xhs2763</t>
+          <t>"Mohamed Alnaqbi"</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
@@ -2927,24 +2927,24 @@
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>3140</t>
+          <t>4937</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>69416</t>
+          <t>24604</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>44378757</t>
+          <t>28855852</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>"NᵉᵗʰᵉʳDʳⁱᶠᵗᵉʳ ㊥"</t>
+          <t>tiger</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
@@ -2954,24 +2954,24 @@
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>2500</t>
+          <t>4910</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>23272</t>
+          <t>26567</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>25479797</t>
+          <t>44708798</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>"Mohamed Alnaqbi"</t>
+          <t>"㊥ mythgod"</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
@@ -2981,24 +2981,24 @@
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>4937</t>
+          <t>4808</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>24324</t>
+          <t>52631</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>37069173</t>
+          <t>54588689</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>詹toniii</t>
+          <t>㊥墨衍枫迹☜</t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
@@ -3008,24 +3008,24 @@
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>4875</t>
+          <t>3127</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>26454</t>
+          <t>26012</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>28855852</t>
+          <t>55634661</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>tiger</t>
+          <t>Opalus</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
@@ -3035,24 +3035,24 @@
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>4766</t>
+          <t>4835</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>26739</t>
+          <t>29418</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>44708798</t>
+          <t>3649043</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>"㊥ mythgod"</t>
+          <t>Dj6106</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
@@ -3062,24 +3062,24 @@
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>4752</t>
+          <t>4673</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>52653</t>
+          <t>30260</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>54588689</t>
+          <t>18082891</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>㊥墨衍枫迹☜</t>
+          <t>Michael</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
@@ -3089,24 +3089,24 @@
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>3098</t>
+          <t>4635</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>8350</t>
+          <t>31759</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>7025661</t>
+          <t>47459684</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>"F ᶻᵍˣ"</t>
+          <t>㊥阿闹切克闹</t>
         </is>
       </c>
       <c r="D102" t="inlineStr">
@@ -3116,24 +3116,24 @@
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t>6078</t>
+          <t>4570</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>22060</t>
+          <t>34570</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>28387448</t>
+          <t>56379103</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>☜⊙‖⊙☞</t>
+          <t>Globalking</t>
         </is>
       </c>
       <c r="D103" t="inlineStr">
@@ -3143,24 +3143,24 @@
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>5008</t>
+          <t>4428</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>26397</t>
+          <t>34770</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>55634661</t>
+          <t>56585361</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>Opalus</t>
+          <t>"㊥ go策划我要ali"</t>
         </is>
       </c>
       <c r="D104" t="inlineStr">
@@ -3170,24 +3170,24 @@
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t>4768</t>
+          <t>4417</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>29333</t>
+          <t>34994</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>18082891</t>
+          <t>58743790</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>Michael</t>
+          <t>Ma</t>
         </is>
       </c>
       <c r="D105" t="inlineStr">
@@ -3197,24 +3197,24 @@
       </c>
       <c r="E105" t="inlineStr">
         <is>
-          <t>4632</t>
+          <t>4405</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>30675</t>
+          <t>35146</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>47459684</t>
+          <t>56732705</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>㊥阿闹切克闹</t>
+          <t>时间温柔皆遗憾</t>
         </is>
       </c>
       <c r="D106" t="inlineStr">
@@ -3224,24 +3224,24 @@
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t>4575</t>
+          <t>4397</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>31866</t>
+          <t>35887</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>3649043</t>
+          <t>58839983</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>Dj6106</t>
+          <t>每逢佳节胖六斤</t>
         </is>
       </c>
       <c r="D107" t="inlineStr">
@@ -3251,24 +3251,24 @@
       </c>
       <c r="E107" t="inlineStr">
         <is>
-          <t>4520</t>
+          <t>4356</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>32962</t>
+          <t>36795</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>58743790</t>
+          <t>55499394</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>Ma</t>
+          <t>Player-55499394</t>
         </is>
       </c>
       <c r="D108" t="inlineStr">
@@ -3278,24 +3278,24 @@
       </c>
       <c r="E108" t="inlineStr">
         <is>
-          <t>4466</t>
+          <t>4306</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>34144</t>
+          <t>37656</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>56379103</t>
+          <t>11645391</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>Globalking</t>
+          <t>"omar omar"</t>
         </is>
       </c>
       <c r="D109" t="inlineStr">
@@ -3305,24 +3305,24 @@
       </c>
       <c r="E109" t="inlineStr">
         <is>
-          <t>4402</t>
+          <t>4262</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>34344</t>
+          <t>39164</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>56732705</t>
+          <t>58408326</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>时间温柔皆遗憾</t>
+          <t>"Killer Bee"</t>
         </is>
       </c>
       <c r="D110" t="inlineStr">
@@ -3332,24 +3332,24 @@
       </c>
       <c r="E110" t="inlineStr">
         <is>
-          <t>4392</t>
+          <t>4184</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>36406</t>
+          <t>42288</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>55499394</t>
+          <t>47244896</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>Player-55499394</t>
+          <t>Dropthebeat</t>
         </is>
       </c>
       <c r="D111" t="inlineStr">
@@ -3359,24 +3359,24 @@
       </c>
       <c r="E111" t="inlineStr">
         <is>
-          <t>4285</t>
+          <t>4014</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>36466</t>
+          <t>42562</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>56585361</t>
+          <t>1304123</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>"㊥ go策划我要ali"</t>
+          <t>Cccccccccccc</t>
         </is>
       </c>
       <c r="D112" t="inlineStr">
@@ -3386,24 +3386,24 @@
       </c>
       <c r="E112" t="inlineStr">
         <is>
-          <t>4282</t>
+          <t>3998</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>37023</t>
+          <t>43715</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>58839983</t>
+          <t>52997727</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>每逢佳节胖六斤</t>
+          <t>larios</t>
         </is>
       </c>
       <c r="D113" t="inlineStr">
@@ -3413,24 +3413,24 @@
       </c>
       <c r="E113" t="inlineStr">
         <is>
-          <t>4254</t>
+          <t>3922</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>39783</t>
+          <t>46354</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>45404911</t>
+          <t>58641574</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>小伙伴666</t>
+          <t>Player-58641574鱼</t>
         </is>
       </c>
       <c r="D114" t="inlineStr">
@@ -3440,24 +3440,24 @@
       </c>
       <c r="E114" t="inlineStr">
         <is>
-          <t>4116</t>
+          <t>3648</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>40676</t>
+          <t>46515</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>58408326</t>
+          <t>48634530</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>"Killer Bee"</t>
+          <t>leezhenrui</t>
         </is>
       </c>
       <c r="D115" t="inlineStr">
@@ -3467,24 +3467,24 @@
       </c>
       <c r="E115" t="inlineStr">
         <is>
-          <t>4071</t>
+          <t>3633</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>41462</t>
+          <t>48502</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>1304123</t>
+          <t>56700848</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>Cccccccccccc</t>
+          <t>工口漫画老师</t>
         </is>
       </c>
       <c r="D116" t="inlineStr">
@@ -3494,24 +3494,24 @@
       </c>
       <c r="E116" t="inlineStr">
         <is>
-          <t>4026</t>
+          <t>3448</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>41526</t>
+          <t>50948</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>47244896</t>
+          <t>58940575</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>Dropthebeat</t>
+          <t>图啊图z z</t>
         </is>
       </c>
       <c r="D117" t="inlineStr">
@@ -3521,24 +3521,24 @@
       </c>
       <c r="E117" t="inlineStr">
         <is>
-          <t>4021</t>
+          <t>3256</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>43017</t>
+          <t>52584</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>48738257</t>
+          <t>52157846</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>死亡洲际跳蛋</t>
+          <t>Hamza</t>
         </is>
       </c>
       <c r="D118" t="inlineStr">
@@ -3548,24 +3548,24 @@
       </c>
       <c r="E118" t="inlineStr">
         <is>
-          <t>3939</t>
+          <t>3130</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>43541</t>
+          <t>58797</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>11645391</t>
+          <t>9718882</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>"omar omar"</t>
+          <t>小霸王2021</t>
         </is>
       </c>
       <c r="D119" t="inlineStr">
@@ -3575,24 +3575,24 @@
       </c>
       <c r="E119" t="inlineStr">
         <is>
-          <t>3892</t>
+          <t>2810</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>43656</t>
+          <t>62298</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>52997727</t>
+          <t>52792063</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>larios</t>
+          <t>"Tramaine Dowlen"</t>
         </is>
       </c>
       <c r="D120" t="inlineStr">
@@ -3602,24 +3602,24 @@
       </c>
       <c r="E120" t="inlineStr">
         <is>
-          <t>3880</t>
+          <t>2681</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>45798</t>
+          <t>62839</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>58641574</t>
+          <t>3391765</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>Player-58641574鱼</t>
+          <t>马er</t>
         </is>
       </c>
       <c r="D121" t="inlineStr">
@@ -3629,24 +3629,24 @@
       </c>
       <c r="E121" t="inlineStr">
         <is>
-          <t>3655</t>
+          <t>2664</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>46442</t>
+          <t>63546</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>48634530</t>
+          <t>47430231</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>leezhenrui</t>
+          <t>Kentantrino</t>
         </is>
       </c>
       <c r="D122" t="inlineStr">
@@ -3656,24 +3656,24 @@
       </c>
       <c r="E122" t="inlineStr">
         <is>
-          <t>3591</t>
+          <t>2643</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>48002</t>
+          <t>63571</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>56700848</t>
+          <t>5367482</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>工口漫画老师</t>
+          <t>Ігор</t>
         </is>
       </c>
       <c r="D123" t="inlineStr">
@@ -3683,24 +3683,24 @@
       </c>
       <c r="E123" t="inlineStr">
         <is>
-          <t>3450</t>
+          <t>2642</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>50384</t>
+          <t>64089</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>58940575</t>
+          <t>15436348</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>图啊图z z</t>
+          <t>Lucas</t>
         </is>
       </c>
       <c r="D124" t="inlineStr">
@@ -3710,24 +3710,24 @@
       </c>
       <c r="E124" t="inlineStr">
         <is>
-          <t>3260</t>
+          <t>2626</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>52075</t>
+          <t>74014</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>52157846</t>
+          <t>20372140</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>Hamza</t>
+          <t>人山即是仙</t>
         </is>
       </c>
       <c r="D125" t="inlineStr">
@@ -3737,24 +3737,24 @@
       </c>
       <c r="E125" t="inlineStr">
         <is>
-          <t>3136</t>
+          <t>2395</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>61847</t>
+          <t>91018</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>52792063</t>
+          <t>57219176</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>"Tramaine Dowlen"</t>
+          <t>青莲道人</t>
         </is>
       </c>
       <c r="D126" t="inlineStr">
@@ -3764,24 +3764,24 @@
       </c>
       <c r="E126" t="inlineStr">
         <is>
-          <t>2682</t>
+          <t>1998</t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>63043</t>
+          <t>95762</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>47430231</t>
+          <t>54941706</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>Kentantrino</t>
+          <t>AlexMenjivar20</t>
         </is>
       </c>
       <c r="D127" t="inlineStr">
@@ -3791,24 +3791,24 @@
       </c>
       <c r="E127" t="inlineStr">
         <is>
-          <t>2645</t>
+          <t>1806</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>63103</t>
+          <t>150588</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>5367482</t>
+          <t>49000199</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>Ігор</t>
+          <t>SlipperyForester5672</t>
         </is>
       </c>
       <c r="D128" t="inlineStr">
@@ -3818,24 +3818,24 @@
       </c>
       <c r="E128" t="inlineStr">
         <is>
-          <t>2643</t>
+          <t>1156</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>63370</t>
+          <t>999999</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>3391765</t>
+          <t>38994054</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>马er</t>
+          <t>chengnan</t>
         </is>
       </c>
       <c r="D129" t="inlineStr">
@@ -3845,24 +3845,24 @@
       </c>
       <c r="E129" t="inlineStr">
         <is>
-          <t>2635</t>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>63603</t>
+          <t>999999</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>15436348</t>
+          <t>55810157</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>Lucas</t>
+          <t>Beard</t>
         </is>
       </c>
       <c r="D130" t="inlineStr">
@@ -3872,24 +3872,24 @@
       </c>
       <c r="E130" t="inlineStr">
         <is>
-          <t>2628</t>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>71446</t>
+          <t>999999</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>9718882</t>
+          <t>57556179</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>小霸王2021</t>
+          <t>特战新生代英雄</t>
         </is>
       </c>
       <c r="D131" t="inlineStr">
@@ -3899,24 +3899,24 @@
       </c>
       <c r="E131" t="inlineStr">
         <is>
-          <t>2467</t>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>73387</t>
+          <t>999999</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>20372140</t>
+          <t>1222440</t>
         </is>
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>人山即是仙</t>
+          <t>"Sneaky Ninja Panda"</t>
         </is>
       </c>
       <c r="D132" t="inlineStr">
@@ -3926,24 +3926,24 @@
       </c>
       <c r="E132" t="inlineStr">
         <is>
-          <t>2398</t>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>90354</t>
+          <t>999999</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>57219176</t>
+          <t>58340439</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>青莲道人</t>
+          <t>70qilin</t>
         </is>
       </c>
       <c r="D133" t="inlineStr">
@@ -3953,24 +3953,24 @@
       </c>
       <c r="E133" t="inlineStr">
         <is>
-          <t>1999</t>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>95800</t>
+          <t>999999</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>54941706</t>
+          <t>58615925</t>
         </is>
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>AlexMenjivar20</t>
+          <t>齐天的大圣</t>
         </is>
       </c>
       <c r="D134" t="inlineStr">
@@ -3980,61 +3980,61 @@
       </c>
       <c r="E134" t="inlineStr">
         <is>
-          <t>1782</t>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>151043</t>
+          <t>51606</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>49000199</t>
+          <t>41849539</t>
         </is>
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>SlipperyForester5672</t>
+          <t>三号馆馆主</t>
         </is>
       </c>
       <c r="D135" t="inlineStr">
         <is>
-          <t>二馆</t>
+          <t>三馆</t>
         </is>
       </c>
       <c r="E135" t="inlineStr">
         <is>
-          <t>1125</t>
+          <t>3207</t>
         </is>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>999999</t>
+          <t>45408</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>38994054</t>
+          <t>56241637</t>
         </is>
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>chengnan</t>
+          <t>Player-14day</t>
         </is>
       </c>
       <c r="D136" t="inlineStr">
         <is>
-          <t>二馆</t>
+          <t>三馆</t>
         </is>
       </c>
       <c r="E136" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>3743</t>
         </is>
       </c>
     </row>
@@ -4046,17 +4046,17 @@
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>55810157</t>
+          <t>47622456</t>
         </is>
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>Beard</t>
+          <t>伊恩</t>
         </is>
       </c>
       <c r="D137" t="inlineStr">
         <is>
-          <t>二馆</t>
+          <t>三馆</t>
         </is>
       </c>
       <c r="E137" t="inlineStr">
@@ -4068,27 +4068,27 @@
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>999999</t>
+          <t>50892</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>57556179</t>
+          <t>55210350</t>
         </is>
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>特战新生代英雄</t>
+          <t>一个过客而已</t>
         </is>
       </c>
       <c r="D138" t="inlineStr">
         <is>
-          <t>二馆</t>
+          <t>三馆</t>
         </is>
       </c>
       <c r="E138" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>3260</t>
         </is>
       </c>
     </row>
@@ -4100,17 +4100,17 @@
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>1222440</t>
+          <t>49553719</t>
         </is>
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>"Sneaky Ninja Panda"</t>
+          <t>"Oreo Captain Sir"</t>
         </is>
       </c>
       <c r="D139" t="inlineStr">
         <is>
-          <t>二馆</t>
+          <t>三馆</t>
         </is>
       </c>
       <c r="E139" t="inlineStr">
@@ -4122,71 +4122,71 @@
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>999999</t>
+          <t>80288</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>58340439</t>
+          <t>59081265</t>
         </is>
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>70qilin</t>
+          <t>爬楼梯</t>
         </is>
       </c>
       <c r="D140" t="inlineStr">
         <is>
-          <t>二馆</t>
+          <t>三馆</t>
         </is>
       </c>
       <c r="E140" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2230</t>
         </is>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>999999</t>
+          <t>82898</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>58615925</t>
+          <t>58671339</t>
         </is>
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>齐天的大圣</t>
+          <t>"quang pro"</t>
         </is>
       </c>
       <c r="D141" t="inlineStr">
         <is>
-          <t>二馆</t>
+          <t>三馆</t>
         </is>
       </c>
       <c r="E141" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2180</t>
         </is>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>51875</t>
+          <t>107019</t>
         </is>
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>41849539</t>
+          <t>59082827</t>
         </is>
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>三号馆馆主</t>
+          <t>Player-59082827</t>
         </is>
       </c>
       <c r="D142" t="inlineStr">
@@ -4196,24 +4196,24 @@
       </c>
       <c r="E142" t="inlineStr">
         <is>
-          <t>3150</t>
+          <t>1580</t>
         </is>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>44785</t>
+          <t>116229</t>
         </is>
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>56241637</t>
+          <t>41231396</t>
         </is>
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t>Player-14day</t>
+          <t>ollsthebro</t>
         </is>
       </c>
       <c r="D143" t="inlineStr">
@@ -4223,7 +4223,7 @@
       </c>
       <c r="E143" t="inlineStr">
         <is>
-          <t>3757</t>
+          <t>1498</t>
         </is>
       </c>
     </row>
@@ -4235,12 +4235,12 @@
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>47622456</t>
+          <t>58572199</t>
         </is>
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t>伊恩</t>
+          <t>你干嘛～哎呦～</t>
         </is>
       </c>
       <c r="D144" t="inlineStr">
@@ -4257,17 +4257,17 @@
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>50334</t>
+          <t>999999</t>
         </is>
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>55210350</t>
+          <t>58766144</t>
         </is>
       </c>
       <c r="C145" t="inlineStr">
         <is>
-          <t>一个过客而已</t>
+          <t>EquablePrecedence38</t>
         </is>
       </c>
       <c r="D145" t="inlineStr">
@@ -4277,7 +4277,7 @@
       </c>
       <c r="E145" t="inlineStr">
         <is>
-          <t>3264</t>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -4289,12 +4289,12 @@
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>49553719</t>
+          <t>29355299</t>
         </is>
       </c>
       <c r="C146" t="inlineStr">
         <is>
-          <t>"Oreo Captain Sir"</t>
+          <t>Player-29355299</t>
         </is>
       </c>
       <c r="D146" t="inlineStr">
@@ -4311,17 +4311,17 @@
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>82225</t>
+          <t>999999</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>58671339</t>
+          <t>58910668</t>
         </is>
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>"quang pro"</t>
+          <t>BrittleAuthor33</t>
         </is>
       </c>
       <c r="D147" t="inlineStr">
@@ -4331,24 +4331,24 @@
       </c>
       <c r="E147" t="inlineStr">
         <is>
-          <t>2180</t>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>92616</t>
+          <t>999999</t>
         </is>
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>59081265</t>
+          <t>55745105</t>
         </is>
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>爬楼梯</t>
+          <t>eldeniz</t>
         </is>
       </c>
       <c r="D148" t="inlineStr">
@@ -4358,24 +4358,24 @@
       </c>
       <c r="E148" t="inlineStr">
         <is>
-          <t>1911</t>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>105603</t>
+          <t>999999</t>
         </is>
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>59082827</t>
+          <t>58174442</t>
         </is>
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>Player-59082827</t>
+          <t>Player-58174442</t>
         </is>
       </c>
       <c r="D149" t="inlineStr">
@@ -4385,88 +4385,88 @@
       </c>
       <c r="E149" t="inlineStr">
         <is>
-          <t>1586</t>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>115172</t>
+          <t>56052</t>
         </is>
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>41231396</t>
+          <t>10636651</t>
         </is>
       </c>
       <c r="C150" t="inlineStr">
         <is>
-          <t>ollsthebro</t>
+          <t>"Ismail Aflou"</t>
         </is>
       </c>
       <c r="D150" t="inlineStr">
         <is>
-          <t>三馆</t>
+          <t>Chinese</t>
         </is>
       </c>
       <c r="E150" t="inlineStr">
         <is>
-          <t>1498</t>
+          <t>2938</t>
         </is>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>999999</t>
+          <t>50218</t>
         </is>
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>58572199</t>
+          <t>41848598</t>
         </is>
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>你干嘛～哎呦～</t>
+          <t>国家一级保护沙雕</t>
         </is>
       </c>
       <c r="D151" t="inlineStr">
         <is>
-          <t>三馆</t>
+          <t>Chinese</t>
         </is>
       </c>
       <c r="E151" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>3310</t>
         </is>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>999999</t>
+          <t>64259</t>
         </is>
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>58766144</t>
+          <t>6010122</t>
         </is>
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>EquablePrecedence38</t>
+          <t>"Edward Peng"</t>
         </is>
       </c>
       <c r="D152" t="inlineStr">
         <is>
-          <t>三馆</t>
+          <t>Chinese</t>
         </is>
       </c>
       <c r="E152" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2620</t>
         </is>
       </c>
     </row>
@@ -4478,17 +4478,17 @@
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>29355299</t>
+          <t>12648101</t>
         </is>
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>Player-29355299</t>
+          <t>"player 198827"</t>
         </is>
       </c>
       <c r="D153" t="inlineStr">
         <is>
-          <t>三馆</t>
+          <t>Chinese</t>
         </is>
       </c>
       <c r="E153" t="inlineStr">
@@ -4505,17 +4505,17 @@
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>58910668</t>
+          <t>9195340</t>
         </is>
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>BrittleAuthor33</t>
+          <t>Namllllllik</t>
         </is>
       </c>
       <c r="D154" t="inlineStr">
         <is>
-          <t>三馆</t>
+          <t>Chinese</t>
         </is>
       </c>
       <c r="E154" t="inlineStr">
@@ -4532,17 +4532,17 @@
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>55745105</t>
+          <t>15755724</t>
         </is>
       </c>
       <c r="C155" t="inlineStr">
         <is>
-          <t>eldeniz</t>
+          <t>"Last Good"</t>
         </is>
       </c>
       <c r="D155" t="inlineStr">
         <is>
-          <t>三馆</t>
+          <t>Chinese</t>
         </is>
       </c>
       <c r="E155" t="inlineStr">
@@ -4559,17 +4559,17 @@
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>58174442</t>
+          <t>8850180</t>
         </is>
       </c>
       <c r="C156" t="inlineStr">
         <is>
-          <t>Player-58174442</t>
+          <t>30624300</t>
         </is>
       </c>
       <c r="D156" t="inlineStr">
         <is>
-          <t>三馆</t>
+          <t>Chinese</t>
         </is>
       </c>
       <c r="E156" t="inlineStr">
@@ -4581,17 +4581,17 @@
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>55593</t>
+          <t>999999</t>
         </is>
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>10636651</t>
+          <t>28624723</t>
         </is>
       </c>
       <c r="C157" t="inlineStr">
         <is>
-          <t>"Ismail Aflou"</t>
+          <t>"Woody Shade"</t>
         </is>
       </c>
       <c r="D157" t="inlineStr">
@@ -4601,24 +4601,24 @@
       </c>
       <c r="E157" t="inlineStr">
         <is>
-          <t>2940</t>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>50570</t>
+          <t>999999</t>
         </is>
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>41848598</t>
+          <t>9913517</t>
         </is>
       </c>
       <c r="C158" t="inlineStr">
         <is>
-          <t>国家一级保护沙雕</t>
+          <t>"Kenny Chan"</t>
         </is>
       </c>
       <c r="D158" t="inlineStr">
@@ -4627,195 +4627,6 @@
         </is>
       </c>
       <c r="E158" t="inlineStr">
-        <is>
-          <t>3248</t>
-        </is>
-      </c>
-    </row>
-    <row r="159">
-      <c r="A159" t="inlineStr">
-        <is>
-          <t>64409</t>
-        </is>
-      </c>
-      <c r="B159" t="inlineStr">
-        <is>
-          <t>6010122</t>
-        </is>
-      </c>
-      <c r="C159" t="inlineStr">
-        <is>
-          <t>"Edward Peng"</t>
-        </is>
-      </c>
-      <c r="D159" t="inlineStr">
-        <is>
-          <t>Chinese</t>
-        </is>
-      </c>
-      <c r="E159" t="inlineStr">
-        <is>
-          <t>2604</t>
-        </is>
-      </c>
-    </row>
-    <row r="160">
-      <c r="A160" t="inlineStr">
-        <is>
-          <t>999999</t>
-        </is>
-      </c>
-      <c r="B160" t="inlineStr">
-        <is>
-          <t>12648101</t>
-        </is>
-      </c>
-      <c r="C160" t="inlineStr">
-        <is>
-          <t>"player 198827"</t>
-        </is>
-      </c>
-      <c r="D160" t="inlineStr">
-        <is>
-          <t>Chinese</t>
-        </is>
-      </c>
-      <c r="E160" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-    </row>
-    <row r="161">
-      <c r="A161" t="inlineStr">
-        <is>
-          <t>999999</t>
-        </is>
-      </c>
-      <c r="B161" t="inlineStr">
-        <is>
-          <t>9195340</t>
-        </is>
-      </c>
-      <c r="C161" t="inlineStr">
-        <is>
-          <t>Namllllllik</t>
-        </is>
-      </c>
-      <c r="D161" t="inlineStr">
-        <is>
-          <t>Chinese</t>
-        </is>
-      </c>
-      <c r="E161" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-    </row>
-    <row r="162">
-      <c r="A162" t="inlineStr">
-        <is>
-          <t>999999</t>
-        </is>
-      </c>
-      <c r="B162" t="inlineStr">
-        <is>
-          <t>15755724</t>
-        </is>
-      </c>
-      <c r="C162" t="inlineStr">
-        <is>
-          <t>"Last Good"</t>
-        </is>
-      </c>
-      <c r="D162" t="inlineStr">
-        <is>
-          <t>Chinese</t>
-        </is>
-      </c>
-      <c r="E162" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-    </row>
-    <row r="163">
-      <c r="A163" t="inlineStr">
-        <is>
-          <t>999999</t>
-        </is>
-      </c>
-      <c r="B163" t="inlineStr">
-        <is>
-          <t>8850180</t>
-        </is>
-      </c>
-      <c r="C163" t="inlineStr">
-        <is>
-          <t>30624300</t>
-        </is>
-      </c>
-      <c r="D163" t="inlineStr">
-        <is>
-          <t>Chinese</t>
-        </is>
-      </c>
-      <c r="E163" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-    </row>
-    <row r="164">
-      <c r="A164" t="inlineStr">
-        <is>
-          <t>999999</t>
-        </is>
-      </c>
-      <c r="B164" t="inlineStr">
-        <is>
-          <t>28624723</t>
-        </is>
-      </c>
-      <c r="C164" t="inlineStr">
-        <is>
-          <t>"Woody Shade"</t>
-        </is>
-      </c>
-      <c r="D164" t="inlineStr">
-        <is>
-          <t>Chinese</t>
-        </is>
-      </c>
-      <c r="E164" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-    </row>
-    <row r="165">
-      <c r="A165" t="inlineStr">
-        <is>
-          <t>999999</t>
-        </is>
-      </c>
-      <c r="B165" t="inlineStr">
-        <is>
-          <t>9913517</t>
-        </is>
-      </c>
-      <c r="C165" t="inlineStr">
-        <is>
-          <t>"Kenny Chan"</t>
-        </is>
-      </c>
-      <c r="D165" t="inlineStr">
-        <is>
-          <t>Chinese</t>
-        </is>
-      </c>
-      <c r="E165" t="inlineStr">
         <is>
           <t>0</t>
         </is>

</xml_diff>